<commit_message>
Update data/tests based on failing unit tests
</commit_message>
<xml_diff>
--- a/common/document_parser/lib/responsibility_parse/tests/data/input/expected_responsibility_results.xlsx
+++ b/common/document_parser/lib/responsibility_parse/tests/data/input/expected_responsibility_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austinmishoe/bah/advana/gamechanger-data/common/document_parser/lib/responsibility_parse/tests/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{549E2916-9082-4146-9FB3-0D9C4E0F6F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D39201-0DBB-1044-9B68-2A3BDCADB745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="262">
   <si>
     <t>filename</t>
   </si>
@@ -800,6 +800,12 @@
   </si>
   <si>
     <t>Implement CLIP requirements within their respective Department’s Active and Reserve</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>active</t>
   </si>
 </sst>
 </file>
@@ -828,7 +834,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -851,13 +857,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1162,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H135"/>
+  <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="D140" sqref="D140"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1173,7 +1193,7 @@
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1198,8 +1218,11 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1224,8 +1247,11 @@
       <c r="H2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1247,8 +1273,11 @@
       <c r="G3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1273,8 +1302,11 @@
       <c r="H4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1296,8 +1328,11 @@
       <c r="G5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1319,8 +1354,11 @@
       <c r="G6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1345,8 +1383,11 @@
       <c r="H7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1371,8 +1412,11 @@
       <c r="H8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1394,8 +1438,11 @@
       <c r="G9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1420,8 +1467,11 @@
       <c r="H10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1443,8 +1493,11 @@
       <c r="G11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1469,8 +1522,11 @@
       <c r="H12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1492,8 +1548,11 @@
       <c r="G13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1515,8 +1574,11 @@
       <c r="G14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1541,8 +1603,11 @@
       <c r="H15" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1564,8 +1629,11 @@
       <c r="G16" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1587,8 +1655,11 @@
       <c r="G17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1613,8 +1684,11 @@
       <c r="H18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1636,8 +1710,11 @@
       <c r="G19" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1659,8 +1736,11 @@
       <c r="G20" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1685,8 +1765,11 @@
       <c r="H21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1708,8 +1791,11 @@
       <c r="G22" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1734,8 +1820,11 @@
       <c r="H23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1760,8 +1849,11 @@
       <c r="H24" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1783,8 +1875,11 @@
       <c r="G25" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1806,8 +1901,11 @@
       <c r="G26" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1832,8 +1930,11 @@
       <c r="H27" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1855,8 +1956,11 @@
       <c r="G28" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1872,8 +1976,11 @@
       <c r="E29" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1895,8 +2002,11 @@
       <c r="G30" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1921,8 +2031,11 @@
       <c r="H31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -1944,8 +2057,11 @@
       <c r="G32" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -1967,8 +2083,11 @@
       <c r="G33" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -1990,8 +2109,11 @@
       <c r="G34" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -2013,8 +2135,11 @@
       <c r="G35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -2036,8 +2161,11 @@
       <c r="G36" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -2059,8 +2187,11 @@
       <c r="G37" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -2082,8 +2213,11 @@
       <c r="G38" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -2108,8 +2242,11 @@
       <c r="H39" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -2134,8 +2271,11 @@
       <c r="H40" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -2160,8 +2300,11 @@
       <c r="H41" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -2186,8 +2329,11 @@
       <c r="H42" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -2209,8 +2355,11 @@
       <c r="G43" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -2232,8 +2381,11 @@
       <c r="G44" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -2255,8 +2407,11 @@
       <c r="G45" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -2281,8 +2436,11 @@
       <c r="H46" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -2304,8 +2462,11 @@
       <c r="G47" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I47" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -2327,8 +2488,11 @@
       <c r="G48" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -2353,8 +2517,11 @@
       <c r="H49" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -2376,8 +2543,11 @@
       <c r="G50" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I50" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -2399,8 +2569,11 @@
       <c r="G51" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -2422,8 +2595,11 @@
       <c r="G52" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>102</v>
       </c>
@@ -2448,8 +2624,11 @@
       <c r="H53" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>102</v>
       </c>
@@ -2474,8 +2653,11 @@
       <c r="H54" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I54" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>102</v>
       </c>
@@ -2500,8 +2682,11 @@
       <c r="H55" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I55" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>102</v>
       </c>
@@ -2523,8 +2708,11 @@
       <c r="G56" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I56" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>102</v>
       </c>
@@ -2549,8 +2737,11 @@
       <c r="H57" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I57" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>102</v>
       </c>
@@ -2575,8 +2766,11 @@
       <c r="H58" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>102</v>
       </c>
@@ -2592,8 +2786,11 @@
       <c r="E59" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I59" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>102</v>
       </c>
@@ -2618,8 +2815,11 @@
       <c r="H60" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>102</v>
       </c>
@@ -2644,8 +2844,11 @@
       <c r="H61" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I61" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>102</v>
       </c>
@@ -2670,8 +2873,11 @@
       <c r="H62" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>102</v>
       </c>
@@ -2693,8 +2899,11 @@
       <c r="G63" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I63" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>102</v>
       </c>
@@ -2719,8 +2928,11 @@
       <c r="H64" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I64" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>102</v>
       </c>
@@ -2745,8 +2957,11 @@
       <c r="H65" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I65" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>102</v>
       </c>
@@ -2771,8 +2986,11 @@
       <c r="H66" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>102</v>
       </c>
@@ -2794,8 +3012,11 @@
       <c r="G67" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I67" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>102</v>
       </c>
@@ -2817,8 +3038,11 @@
       <c r="G68" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I68" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>102</v>
       </c>
@@ -2843,8 +3067,11 @@
       <c r="H69" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I69" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>102</v>
       </c>
@@ -2866,8 +3093,11 @@
       <c r="G70" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>102</v>
       </c>
@@ -2889,8 +3119,11 @@
       <c r="G71" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>102</v>
       </c>
@@ -2912,8 +3145,11 @@
       <c r="G72" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I72" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>102</v>
       </c>
@@ -2938,8 +3174,11 @@
       <c r="H73" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I73" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>102</v>
       </c>
@@ -2961,8 +3200,11 @@
       <c r="G74" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I74" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>102</v>
       </c>
@@ -2987,8 +3229,11 @@
       <c r="H75" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I75" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>102</v>
       </c>
@@ -3010,8 +3255,11 @@
       <c r="G76" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I76" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>102</v>
       </c>
@@ -3033,8 +3281,11 @@
       <c r="G77" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I77" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>102</v>
       </c>
@@ -3059,8 +3310,11 @@
       <c r="H78" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I78" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>102</v>
       </c>
@@ -3082,8 +3336,11 @@
       <c r="G79" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I79" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>102</v>
       </c>
@@ -3105,8 +3362,11 @@
       <c r="G80" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I80" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>102</v>
       </c>
@@ -3131,8 +3391,11 @@
       <c r="H81" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I81" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>102</v>
       </c>
@@ -3154,8 +3417,11 @@
       <c r="G82" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I82" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>102</v>
       </c>
@@ -3177,8 +3443,11 @@
       <c r="G83" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I83" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>102</v>
       </c>
@@ -3203,8 +3472,11 @@
       <c r="H84" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I84" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>102</v>
       </c>
@@ -3226,8 +3498,11 @@
       <c r="G85" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I85" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>102</v>
       </c>
@@ -3252,8 +3527,11 @@
       <c r="H86" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I86" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>102</v>
       </c>
@@ -3278,8 +3556,11 @@
       <c r="H87" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I87" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>102</v>
       </c>
@@ -3304,8 +3585,11 @@
       <c r="H88" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I88" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>102</v>
       </c>
@@ -3330,8 +3614,11 @@
       <c r="H89" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I89" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>102</v>
       </c>
@@ -3356,8 +3643,11 @@
       <c r="H90" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I90" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>102</v>
       </c>
@@ -3382,8 +3672,11 @@
       <c r="H91" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I91" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>102</v>
       </c>
@@ -3405,8 +3698,11 @@
       <c r="G92" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I92" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>102</v>
       </c>
@@ -3428,8 +3724,11 @@
       <c r="G93" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I93" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>102</v>
       </c>
@@ -3451,8 +3750,11 @@
       <c r="G94" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I94" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>102</v>
       </c>
@@ -3477,8 +3779,11 @@
       <c r="H95" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I95" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>102</v>
       </c>
@@ -3503,8 +3808,11 @@
       <c r="H96" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I96" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>102</v>
       </c>
@@ -3529,8 +3837,11 @@
       <c r="H97" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I97" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>102</v>
       </c>
@@ -3555,8 +3866,11 @@
       <c r="H98" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I98" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>102</v>
       </c>
@@ -3581,8 +3895,11 @@
       <c r="H99" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I99" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>102</v>
       </c>
@@ -3604,8 +3921,11 @@
       <c r="G100" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I100" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>102</v>
       </c>
@@ -3627,8 +3947,11 @@
       <c r="G101" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I101" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>102</v>
       </c>
@@ -3650,8 +3973,11 @@
       <c r="G102" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I102" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -3673,8 +3999,11 @@
       <c r="G103" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I103" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -3699,8 +4028,11 @@
       <c r="H104" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I104" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>102</v>
       </c>
@@ -3725,8 +4057,11 @@
       <c r="H105" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I105" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>102</v>
       </c>
@@ -3751,8 +4086,11 @@
       <c r="H106" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I106" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>102</v>
       </c>
@@ -3774,8 +4112,11 @@
       <c r="G107" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I107" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>102</v>
       </c>
@@ -3800,8 +4141,11 @@
       <c r="H108" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I108" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>102</v>
       </c>
@@ -3823,8 +4167,11 @@
       <c r="G109" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I109" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>102</v>
       </c>
@@ -3846,8 +4193,11 @@
       <c r="G110" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I110" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>102</v>
       </c>
@@ -3869,8 +4219,11 @@
       <c r="G111" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I111" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>102</v>
       </c>
@@ -3892,8 +4245,11 @@
       <c r="G112" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I112" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>102</v>
       </c>
@@ -3915,8 +4271,11 @@
       <c r="G113" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I113" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>102</v>
       </c>
@@ -3938,8 +4297,11 @@
       <c r="G114" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I114" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>102</v>
       </c>
@@ -3961,8 +4323,11 @@
       <c r="G115" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I115" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>102</v>
       </c>
@@ -3984,8 +4349,11 @@
       <c r="G116" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I116" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>102</v>
       </c>
@@ -4010,8 +4378,11 @@
       <c r="H117" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I117" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>102</v>
       </c>
@@ -4036,8 +4407,11 @@
       <c r="H118" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I118" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>102</v>
       </c>
@@ -4059,8 +4433,11 @@
       <c r="G119" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I119" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>102</v>
       </c>
@@ -4082,8 +4459,11 @@
       <c r="G120" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I120" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>102</v>
       </c>
@@ -4108,8 +4488,11 @@
       <c r="H121" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I121" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>102</v>
       </c>
@@ -4134,8 +4517,11 @@
       <c r="H122" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I122" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>102</v>
       </c>
@@ -4157,8 +4543,11 @@
       <c r="G123" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I123" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>102</v>
       </c>
@@ -4180,8 +4569,11 @@
       <c r="G124" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I124" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>102</v>
       </c>
@@ -4206,8 +4598,11 @@
       <c r="H125" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I125" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>102</v>
       </c>
@@ -4229,8 +4624,11 @@
       <c r="G126" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I126" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>102</v>
       </c>
@@ -4252,8 +4650,11 @@
       <c r="G127" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I127" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>102</v>
       </c>
@@ -4278,8 +4679,11 @@
       <c r="H128" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I128" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>102</v>
       </c>
@@ -4304,8 +4708,11 @@
       <c r="H129" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I129" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>102</v>
       </c>
@@ -4327,8 +4734,11 @@
       <c r="G130" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I130" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>242</v>
       </c>
@@ -4353,8 +4763,11 @@
       <c r="H131" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I131" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>242</v>
       </c>
@@ -4379,8 +4792,11 @@
       <c r="H132" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I132" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>242</v>
       </c>
@@ -4402,8 +4818,11 @@
       <c r="G133" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I133" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>242</v>
       </c>
@@ -4428,8 +4847,11 @@
       <c r="H134" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I134" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>242</v>
       </c>
@@ -4450,6 +4872,9 @@
       </c>
       <c r="G135" t="s">
         <v>259</v>
+      </c>
+      <c r="I135" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to responsibility parser based on PR feedback
</commit_message>
<xml_diff>
--- a/common/document_parser/lib/responsibility_parse/tests/data/input/expected_responsibility_results.xlsx
+++ b/common/document_parser/lib/responsibility_parse/tests/data/input/expected_responsibility_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:I139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6460,11 +6460,187 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>Implement CLIP requirements within their respective Department’s Active and Reserve</t>
+          <t>Implement CLIP requirements within their respective Department’s Active and Reserve Components and facilities under their supervision to include oversight, inspections, proficiency testing, personnel standards, and training in laboratories performing testing on human specimens as defined under “laboratory” in the Glossary of this instruction.</t>
         </is>
       </c>
       <c r="H135" t="inlineStr"/>
       <c r="I135" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>DoDI 6440.02 CH 1.pdf</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Clinical Laboratory Improvement Program (CLIP)</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>SECRETARIES OF THE MILITARY DEPARTMENTS.  The Secretaries of the Military Departments:</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Military Departments</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>b.</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>In accordance with DoD Manual 6440.02 (Reference (g)), follow CLIP procedures for corrective action on laboratory facilities whose proficiency testing or performance criteria fall outside the standards of CLIP policy.</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>DoD</t>
+        </is>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>DoDI 6440.02 CH 1.pdf</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Clinical Laboratory Improvement Program (CLIP)</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>SECRETARIES OF THE MILITARY DEPARTMENTS.  The Secretaries of the Military Departments:</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Military Departments</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>c.</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>In accordance with Reference (g), implement the standards and procedures governing the operation, management, and oversight of clinical laboratory assets assigned to operational forces. Except where operational constraints preclude compliance, the standards governing clinical laboratory assets assigned to operational forces will incorporate the CLIP policy to the maximum extent possible without impeding operational requirements.</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr"/>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>DoDI 6440.02 CH 1.pdf</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Clinical Laboratory Improvement Program (CLIP)</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>SECRETARIES OF THE MILITARY DEPARTMENTS.  The Secretaries of the Military Departments:</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Military Departments</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>d.</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>Recommend changes and revisions to CLIP standards to CCLM. ENCLOSURE 2</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr"/>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>DoDI 6440.02 CH 1.pdf</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Clinical Laboratory Improvement Program (CLIP)</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>SECRETARIES OF THE MILITARY DEPARTMENTS.  The Secretaries of the Military Departments:</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Military Departments</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>e.</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>Oversee Surgeon General, laboratory commander, and laboratory medical director implementation of the procedures in Enclosure 3 of this instruction.</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr"/>
+      <c r="I139" t="inlineStr">
         <is>
           <t>active</t>
         </is>

</xml_diff>

<commit_message>
Updates to unit tests (add coverage) remove some unused variables in resp parser and add back in `is_larger_numbering` functionality
</commit_message>
<xml_diff>
--- a/common/document_parser/lib/responsibility_parse/tests/data/input/expected_responsibility_results.xlsx
+++ b/common/document_parser/lib/responsibility_parse/tests/data/input/expected_responsibility_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I139"/>
+  <dimension ref="A1:I140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2151,11 +2151,7 @@
           <t>Provide guidance and requirements oversight on whether the MILDEP or Defense Agency workforce is properly educated, trained, and certified for robotic systems, in accordance with a common set of requirements to address appropriate classroom and hands-on training.</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Defense Agency</t>
-        </is>
-      </c>
+      <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr">
         <is>
           <t>active</t>
@@ -4714,11 +4710,7 @@
           <t>Provides procedures and guidance for military postal activities ensuring that all U.S. citizens, with or without Military Post Office privileges, are authorized to mail balloting material from any Military Post Office.</t>
         </is>
       </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>Office</t>
-        </is>
-      </c>
+      <c r="H96" t="inlineStr"/>
       <c r="I96" t="inlineStr">
         <is>
           <t>active</t>
@@ -6445,25 +6437,29 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
+          <t>DIRECTOR, DHA. Under the authority, direction, and control of the ASD(HA):</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>ASDHA;DHA</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
           <t>SECRETARIES OF THE MILITARY DEPARTMENTS.  The Secretaries of the Military Departments:</t>
         </is>
       </c>
-      <c r="E135" t="inlineStr">
+      <c r="H135" t="inlineStr">
         <is>
           <t>Military Departments</t>
         </is>
       </c>
-      <c r="F135" t="inlineStr">
-        <is>
-          <t>a.</t>
-        </is>
-      </c>
-      <c r="G135" t="inlineStr">
-        <is>
-          <t>Implement CLIP requirements within their respective Department’s Active and Reserve Components and facilities under their supervision to include oversight, inspections, proficiency testing, personnel standards, and training in laboratories performing testing on human specimens as defined under “laboratory” in the Glossary of this instruction.</t>
-        </is>
-      </c>
-      <c r="H135" t="inlineStr"/>
       <c r="I135" t="inlineStr">
         <is>
           <t>active</t>
@@ -6488,29 +6484,25 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>SECRETARIES OF THE MILITARY DEPARTMENTS.  The Secretaries of the Military Departments:</t>
+          <t>DIRECTOR, DHA. Under the authority, direction, and control of the ASD(HA):</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Military Departments</t>
+          <t>ASDHA;DHA</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>b.</t>
+          <t>a.</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>In accordance with DoD Manual 6440.02 (Reference (g)), follow CLIP procedures for corrective action on laboratory facilities whose proficiency testing or performance criteria fall outside the standards of CLIP policy.</t>
-        </is>
-      </c>
-      <c r="H136" t="inlineStr">
-        <is>
-          <t>DoD</t>
-        </is>
-      </c>
+          <t>Implement CLIP requirements within their respective Department’s Active and Reserve Components and facilities under their supervision to include oversight, inspections, proficiency testing, personnel standards, and training in laboratories performing testing on human specimens as defined under “laboratory” in the Glossary of this instruction.</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr"/>
       <c r="I136" t="inlineStr">
         <is>
           <t>active</t>
@@ -6535,25 +6527,29 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>SECRETARIES OF THE MILITARY DEPARTMENTS.  The Secretaries of the Military Departments:</t>
+          <t>DIRECTOR, DHA. Under the authority, direction, and control of the ASD(HA):</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Military Departments</t>
+          <t>ASDHA;DHA</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>c.</t>
+          <t>b.</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>In accordance with Reference (g), implement the standards and procedures governing the operation, management, and oversight of clinical laboratory assets assigned to operational forces. Except where operational constraints preclude compliance, the standards governing clinical laboratory assets assigned to operational forces will incorporate the CLIP policy to the maximum extent possible without impeding operational requirements.</t>
-        </is>
-      </c>
-      <c r="H137" t="inlineStr"/>
+          <t>In accordance with DoD Manual 6440.02 (Reference (g)), follow CLIP procedures for corrective action on laboratory facilities whose proficiency testing or performance criteria fall outside the standards of CLIP policy.</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>DoD</t>
+        </is>
+      </c>
       <c r="I137" t="inlineStr">
         <is>
           <t>active</t>
@@ -6578,22 +6574,22 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>SECRETARIES OF THE MILITARY DEPARTMENTS.  The Secretaries of the Military Departments:</t>
+          <t>DIRECTOR, DHA. Under the authority, direction, and control of the ASD(HA):</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Military Departments</t>
+          <t>ASDHA;DHA</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>d.</t>
+          <t>c.</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>Recommend changes and revisions to CLIP standards to CCLM. ENCLOSURE 2</t>
+          <t>In accordance with Reference (g), implement the standards and procedures governing the operation, management, and oversight of clinical laboratory assets assigned to operational forces. Except where operational constraints preclude compliance, the standards governing clinical laboratory assets assigned to operational forces will incorporate the CLIP policy to the maximum extent possible without impeding operational requirements.</t>
         </is>
       </c>
       <c r="H138" t="inlineStr"/>
@@ -6621,26 +6617,69 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>SECRETARIES OF THE MILITARY DEPARTMENTS.  The Secretaries of the Military Departments:</t>
+          <t>DIRECTOR, DHA. Under the authority, direction, and control of the ASD(HA):</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Military Departments</t>
+          <t>ASDHA;DHA</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>e.</t>
+          <t>d.</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>Oversee Surgeon General, laboratory commander, and laboratory medical director implementation of the procedures in Enclosure 3 of this instruction.</t>
+          <t>Recommend changes and revisions to CLIP standards to CCLM. ENCLOSURE 2</t>
         </is>
       </c>
       <c r="H139" t="inlineStr"/>
       <c r="I139" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>DoDI 6440.02 CH 1.pdf</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Clinical Laboratory Improvement Program (CLIP)</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>DIRECTOR, DHA. Under the authority, direction, and control of the ASD(HA):</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>ASDHA;DHA</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>e.</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>Oversee Surgeon General, laboratory commander, and laboratory medical director implementation of the procedures in Enclosure 3 of this instruction.</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr"/>
+      <c r="I140" t="inlineStr">
         <is>
           <t>active</t>
         </is>

</xml_diff>